<commit_message>
updated Scrum artifacts and presentation
</commit_message>
<xml_diff>
--- a/Product Backlog and Sprints.xlsx
+++ b/Product Backlog and Sprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bureauveritas-my.sharepoint.com/personal/joshua_stuckey_bureauveritas_com/Documents/Documents/Python/Projects/Mjolnir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="11_F25DC773A252ABDACC104879D11961DA5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{594B3E9F-6846-4A12-A59E-1AED4232FA00}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="11_F25DC773A252ABDACC104879D11961DA5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE8DDEFF-9095-4002-8085-731F8F788AB5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$12</definedName>
     <definedName name="sprint">Sheet1!XFD:XFD</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Task</t>
   </si>
@@ -90,10 +91,13 @@
     <t>No</t>
   </si>
   <si>
-    <t>Updated README</t>
-  </si>
-  <si>
     <t>Full Documentation overhaul of scripts</t>
+  </si>
+  <si>
+    <t>Updated README for MVP</t>
+  </si>
+  <si>
+    <t>Automate Backlog Spreadsheet with Sprint Tabs</t>
   </si>
 </sst>
 </file>
@@ -129,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -139,6 +143,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,17 +431,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="50.453125" style="1" customWidth="1"/>
     <col min="2" max="4" width="8.7265625" style="3"/>
-    <col min="5" max="6" width="8.7265625" style="2"/>
+    <col min="5" max="5" width="8.7265625" style="2"/>
+    <col min="6" max="6" width="9.453125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -459,97 +467,115 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45912</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3">
         <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45912</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C7" s="3">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>19</v>
@@ -557,13 +583,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>19</v>
@@ -571,21 +597,21 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
@@ -597,7 +623,26 @@
         <v>19</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F12" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F12">
+      <sortCondition ref="E1:E12"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added .py download and extraction scripts, update to scrum excel
</commit_message>
<xml_diff>
--- a/Product Backlog and Sprints.xlsx
+++ b/Product Backlog and Sprints.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bureauveritas-my.sharepoint.com/personal/joshua_stuckey_bureauveritas_com/Documents/Documents/Python/Projects/Mjolnir/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jstuckey\OneDrive - Bureau Veritas\Documents\Python\Projects\Mjolnir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="11_F25DC773A252ABDACC104879D11961DA5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE8DDEFF-9095-4002-8085-731F8F788AB5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CE958A-B4C3-48E4-A75B-840851190840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$12</definedName>
-    <definedName name="sprint">Sheet1!XFD:XFD</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$A$1:$F$12</definedName>
+    <definedName name="sprint">'Product Backlog'!XFD:XFD</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Automate Backlog Spreadsheet with Sprint Tabs</t>
+  </si>
+  <si>
+    <t>Update thunder data analysis to use a centered moving 10 year average</t>
+  </si>
+  <si>
+    <t>Refactor analysis scripts to include station ID in data</t>
   </si>
 </sst>
 </file>
@@ -162,10 +168,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,15 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="8.7265625" style="3"/>
     <col min="5" max="5" width="8.7265625" style="2"/>
     <col min="6" max="6" width="9.453125" style="2" bestFit="1" customWidth="1"/>
@@ -538,13 +540,16 @@
       <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3">
         <v>13</v>
@@ -552,44 +557,53 @@
       <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>45917</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C9" s="3">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>19</v>
@@ -597,10 +611,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3">
         <v>8</v>
@@ -611,13 +625,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>19</v>
@@ -625,21 +639,49 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="3">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3">
+        <v>21</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F12">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
       <sortCondition ref="E1:E12"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
replaced thunder analysis scripts with .py and a placeholder .py for average calculations; updates to presentation and README to reflect new scripts
</commit_message>
<xml_diff>
--- a/Product Backlog and Sprints.xlsx
+++ b/Product Backlog and Sprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jstuckey\OneDrive - Bureau Veritas\Documents\Python\Projects\Mjolnir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CE958A-B4C3-48E4-A75B-840851190840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3FF83E-2968-4E20-9ABD-7FDD3BBC5C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Convert Scraping and Analysis Scripts from Jupyter to .py</t>
-  </si>
-  <si>
     <t>$$</t>
   </si>
   <si>
@@ -104,6 +101,18 @@
   </si>
   <si>
     <t>Refactor analysis scripts to include station ID in data</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Convert Scraping Scripts from Jupyter to .py</t>
+  </si>
+  <si>
+    <t>Convert Thunder analysis scripts from Jupyter to .py</t>
+  </si>
+  <si>
+    <t>Convert Meteorite analysis scripts from Jupyter to .py</t>
   </si>
 </sst>
 </file>
@@ -433,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,9 +454,10 @@
     <col min="2" max="4" width="8.7265625" style="3"/>
     <col min="5" max="5" width="8.7265625" style="2"/>
     <col min="6" max="6" width="9.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +468,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -466,19 +476,22 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -487,18 +500,18 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3">
         <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -507,18 +520,18 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -527,35 +540,38 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="C5" s="3">
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" s="4">
+        <v>45918</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3">
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -564,124 +580,164 @@
         <v>45917</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3">
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7" s="4">
+        <v>45918</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="C8" s="3">
         <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3">
         <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C13" s="3">
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3">
         <v>8</v>
       </c>
-      <c r="C14" s="3">
-        <v>21</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>19</v>
+      <c r="D16" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F16">
       <sortCondition ref="E1:E12"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
update to backlog doc
</commit_message>
<xml_diff>
--- a/Product Backlog and Sprints.xlsx
+++ b/Product Backlog and Sprints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jstuckey\OneDrive - Bureau Veritas\Documents\Python\Projects\Mjolnir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jstuckey\Python\Mjolnir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3FF83E-2968-4E20-9ABD-7FDD3BBC5C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6321BAD-7697-419E-B7B1-C67834F920D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Updated README for MVP</t>
   </si>
   <si>
-    <t>Automate Backlog Spreadsheet with Sprint Tabs</t>
-  </si>
-  <si>
     <t>Update thunder data analysis to use a centered moving 10 year average</t>
   </si>
   <si>
@@ -113,6 +110,9 @@
   </si>
   <si>
     <t>Convert Meteorite analysis scripts from Jupyter to .py</t>
+  </si>
+  <si>
+    <t>in progress, thunder_averages.py being actively worked on</t>
   </si>
 </sst>
 </file>
@@ -148,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -161,6 +161,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,7 +457,7 @@
     <col min="2" max="4" width="8.7265625" style="3"/>
     <col min="5" max="5" width="8.7265625" style="2"/>
     <col min="6" max="6" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -476,8 +479,8 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>24</v>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -542,7 +545,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -582,7 +585,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
@@ -602,7 +605,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
@@ -622,7 +625,7 @@
     </row>
     <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -636,10 +639,13 @@
       <c r="E9" s="2">
         <v>3</v>
       </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -718,20 +724,6 @@
         <v>21</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3">
-        <v>8</v>
-      </c>
-      <c r="D16" s="3" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
backlog update and final thunder averages script
</commit_message>
<xml_diff>
--- a/Product Backlog and Sprints.xlsx
+++ b/Product Backlog and Sprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jstuckey\Python\Mjolnir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6321BAD-7697-419E-B7B1-C67834F920D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68307B3C-B7D4-4845-BA80-4C75BC8567BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -112,7 +112,7 @@
     <t>Convert Meteorite analysis scripts from Jupyter to .py</t>
   </si>
   <si>
-    <t>in progress, thunder_averages.py being actively worked on</t>
+    <t>Handle Leap years in Thunder Average Script</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -639,8 +639,8 @@
       <c r="E9" s="2">
         <v>3</v>
       </c>
-      <c r="G9" t="s">
-        <v>27</v>
+      <c r="F9" s="4">
+        <v>45936</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -656,6 +656,9 @@
       <c r="D10" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -724,6 +727,20 @@
         <v>21</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3">
+        <v>13</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>